<commit_message>
Actualización de la version 4 de la matriz HU
</commit_message>
<xml_diff>
--- a/PREGAME/1. ELICITACIÓN/1.3 Historias de Usuario/Matriz HU Grupo 1 V4.0.0.xlsx
+++ b/PREGAME/1. ELICITACIÓN/1.3 Historias de Usuario/Matriz HU Grupo 1 V4.0.0.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\QUINTO SEMESTRE MAYO 23 - SEPTIEMBRE 23\NahirCarrera_14765_G1_MPSW\PREGAME\1. ELICITACIÓN\1.3 Historias de Usuario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noobp\Desktop\semestre 3-4\Modelos de procesos\acabados\NahirCarrera_14765_G1_MPSW\PREGAME\1. ELICITACIÓN\1.3 Historias de Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B196BF4C-52F8-4B40-9818-14D8583DE164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
     <sheet name="Formato descripción HU" sheetId="1" r:id="rId2"/>
     <sheet name="Historia de Usuario" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,12 +119,6 @@
     <t xml:space="preserve">El sistema debe permitir al usuario actualizar su información a su preferencia. </t>
   </si>
   <si>
-    <t>Implementar una funcionalidad de actualización de usuario que permita al usuario modificar tanto su nombre de usuario y su contraseña como sueldo base, garantizando la seguridad y autenticidad del proceso.</t>
-  </si>
-  <si>
-    <t>* Diseñar una interfaz que permita al usuario ingresar y confirmar sus credenciales (nombre de usuario, contraseña, sueldo base) * Desarrollar un proceso de validación que verifique la autenticidad de la actualización de credenciales.</t>
-  </si>
-  <si>
     <t>REQ005</t>
   </si>
   <si>
@@ -205,9 +198,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Proporcionar una experiencia de usuario fluida y personalizable en la visualización del perfil del usuario.</t>
-  </si>
-  <si>
-    <t>En el aplicativo los usuarios podrán verificar su información de manera intuitiva y adaptada a sus preferencias.</t>
   </si>
   <si>
     <t>* Diseñar una interfaz de usuario clara y accesible.
@@ -216,28 +206,9 @@
 * Facilitar la navegación y la edición del perfil.</t>
   </si>
   <si>
-    <t>* Pruebas de usabilidad para evaluar la facilidad de navegación y comprensión de la interfaz del perfil.
-* Pruebas de personalización para confirmar que los usuarios pueden modificar y ajustar la información según sus preferencias.
-* Evaluación de la organización de los elementos del perfil para asegurar una presentación coherente y lógica.
-* Comprobación de las opciones de privacidad y seguridad para garantizar que los usuarios puedan controlar quién accede a su información.
-* Verificación de la funcionalidad de navegación y edición del perfil en diferentes dispositivos y navegadores para asegurar una experiencia consistente.</t>
-  </si>
-  <si>
     <t>El sistema debe facilitar la visualización del listado de materiales de forma clara y accesible para los usuarios.</t>
   </si>
   <si>
-    <t>La implementación de una interfaz intuitiva y estructurada permite a los usuarios acceder al listado de materiales de manera eficaz, facilitando la gestión y el acceso a los recursos necesarios.</t>
-  </si>
-  <si>
-    <t>Verificar la eficacia de la visualización del listado de materiales a través de pruebas de usabilidad y retroalimentación de los usuarios.</t>
-  </si>
-  <si>
-    <t>* Diseñar una interfaz de usuario clara y organizada para mostrar el listado de materiales.
-* Implementar funciones de búsqueda y filtrado para facilitar la navegación.
-* Organizar los materiales de manera jerárquica o categorizada para una mejor comprensión.
-* Proporcionar opciones de visualización personalizables para adaptarse a las preferencias del usuario.</t>
-  </si>
-  <si>
     <t>Añadir materiales</t>
   </si>
   <si>
@@ -247,22 +218,10 @@
     <t>Verificar la funcionalidad de añadir materiales mediante pruebas de ingreso de datos y comprobación de que los nuevos materiales se reflejen correctamente en la base de datos del sistema.</t>
   </si>
   <si>
-    <t>La implementación de  añadir materiales permite a los usuarios contribuir con nuevos recursos al sistema de manera eficiente, asegurando que la base de datos esté actualizada y completa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Diseñar un formulario claro y fácil de entender para la entrada de información del material.
-* Validar la información ingresada para garantizar su precisión y coherencia.
-* Permitir a los usuarios revisar y confirmar la información antes de añadir el material al sistema.
-</t>
-  </si>
-  <si>
     <t>Buscar material</t>
   </si>
   <si>
     <t>El sistema debe facilitar la búsqueda de materiales de manera eficiente y precisa.</t>
-  </si>
-  <si>
-    <t>Permitirá a los usuarios encontrar rápidamente los materiales deseados, mejorando así la eficiencia y la experiencia del usuario.</t>
   </si>
   <si>
     <t>* Diseñar una barra de búsqueda visible y accesible en la interfaz del usuario.
@@ -270,28 +229,10 @@
 * Mostrar resultados de búsqueda relevantes de manera clara y ordenada.</t>
   </si>
   <si>
-    <t>* Introducir un término de búsqueda en la barra de búsqueda.
-* Verificar que los resultados coincidan con el término ingresado.
-* Probar diferentes términos de búsqueda para asegurar la precisión y la amplitud de los resultados.
-* Comprobar la funcionalidad de los filtros y opciones de ordenación para refinar los resultados según las necesidades del usuario.</t>
-  </si>
-  <si>
     <t>Actualización de materiales</t>
   </si>
   <si>
     <t>El sistema debe permitir a los usuarios actualizar la información de los materiales de manera precisa y oportuna.</t>
-  </si>
-  <si>
-    <t>* Diseñar una interfaz de usuario intuitiva que permita la edición de la información del material.
-* Proporcionar opciones para modificar campos específicos del material, como título, descripción, categoría, etc.
-* Validar los cambios realizados para garantizar la coherencia y precisión de la información.
-* Guardar los cambios de manera segura y actualizar la base de datos del sistema con la información actualizada del material.</t>
-  </si>
-  <si>
-    <t>* Seleccionar un material existente para actualizar.
-* Modificar elcampo de información del material.
-* Guardar los cambios realizados.
-* Verificar que los cambios se reflejen correctamente en la interfaz del usuario y en la base de datos del sistema.</t>
   </si>
   <si>
     <t xml:space="preserve"> Eliminación de materiales.</t>
@@ -306,53 +247,18 @@
 * Actualizar la base de datos del sistema eliminando de manera permanente los materiales seleccionados.</t>
   </si>
   <si>
-    <t>* Seleccionar un material para eliminar.
-* Confirmar la eliminación del material.
-* Verificar que el material eliminado ya no esté disponible en la base de datos.
-* Comprobar que los enlaces o referencias al material eliminado se actualicen correctamente en el sistema.</t>
-  </si>
-  <si>
     <t>Visualización del listado de productos</t>
   </si>
   <si>
     <t>El sistema debe permitir a los usuarios visualizar el listado de productos de manera clara y accesible.</t>
   </si>
   <si>
-    <t>* Diseñar una interfaz de usuario que muestre de manera clara y organizada la lista de productos.
-* Incluir información relevante de los productos, como nombre, descripción, precio, disponibilidad, etc.
-* Implementar funciones de búsqueda y filtrado para ayudar a los usuarios a encontrar productos específicos.</t>
-  </si>
-  <si>
-    <t>* Acceder a la página de visualización del listado de productos.
-* Verificar que todos los productos estén listados y sean visibles.
-* Realizar una búsqueda de un producto específico utilizando la función de búsqueda.
-* Aplicar filtros de categoría o precio y verificar que los resultados se actualicen correctamente.
-* Confirmar que la información de cada producto sea precisa y esté completa.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Añadir productos</t>
   </si>
   <si>
     <t>El sistema debe facilitar la incorporación de nuevos productos de manera eficiente y precisa.</t>
   </si>
   <si>
-    <t>El administrador de la tienda necesita la capacidad de agregar nuevos productos al inventario de manera rápida y precisa para mantener actualizado el catálogo de productos disponibles.</t>
-  </si>
-  <si>
-    <t>Permite a los administradores ingresar la información relevante de los nuevos productos de manera eficiente, garantizando así la disponibilidad y precisión del inventario.</t>
-  </si>
-  <si>
-    <t>* Diseñar un formulario de entrada de productos que incluya campos para nombre, descripción, precio, etc.
-* Validar la información ingresada para asegurar su precisión y coherencia.
-* Implementar controles de seguridad para garantizar que solo los administradores autorizados puedan agregar productos.</t>
-  </si>
-  <si>
-    <t>* Acceder al formulario de añadir productos.
-* Ingresar los detalles del nuevo producto, como nombre, descripción, precio, etc.
-* Guardar la información del producto.
-* Verificar que el nuevo producto aparezca correctamente en el catálogo de productos de la tienda.</t>
-  </si>
-  <si>
     <t>Buscar producto</t>
   </si>
   <si>
@@ -377,9 +283,6 @@
     <t>El adminstrador necesita la capacidad de ver una lista completa de productos disponibles en el sistema para verificar compras informadas y tomar decisiones de manera efectiva.</t>
   </si>
   <si>
-    <t>El administrador necesita la capacidad de encontrar rápidamente productos específicos dentro del catálogo de la tienda para facilitar cualquier proceso.</t>
-  </si>
-  <si>
     <t>Permitir al administrador actualizar su información cuando lo desee,  proporcionando flexibilidad y control sobre sus datos.  La falta de esta funcionalidad limita la capacidad de los usuarios para gestionar y personalizar sus credenciales de acceso.</t>
   </si>
   <si>
@@ -392,70 +295,16 @@
     <t>Implementar una función de búsqueda de productos permite al administrador localizar rápidamente los productos deseados.</t>
   </si>
   <si>
-    <t>Implementar una interfaz intuitiva de visualización de listado de productos permite a los usuarios acceder fácilmente a la información relevante de los productos, facilitando así la navegación.</t>
-  </si>
-  <si>
-    <t>* Diseñar una barra de búsqueda prominente en la interfaz del administrador.
-* Implementar algoritmos de búsqueda eficientes que permitan la búsqueda por nombre, categoría, precio, etc.
-* Mostrar resultados de búsqueda relevantes de manera clara y ordenada.
-* Proporcionar opciones de filtrado y ordenación para refinar los resultados de búsqueda.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-* Ingresar un término de búsqueda en la barra de búsqueda.
-* Verificar que los resultados de búsqueda coincidan con el término ingresado.
-* Probar diferentes términos de búsqueda para asegurar la precisión y la amplitud de los resultados.
-* Comprobar la funcionalidad de los filtros y opciones de ordenación para refinar los resultados según las necesidades del administrador.</t>
-  </si>
-  <si>
     <t>Actualización del producto</t>
   </si>
   <si>
     <t>El sistema debe permitir al administrador actualizar la información de los productos de manera efectiva y oportuna.</t>
   </si>
   <si>
-    <t>El administrador necesita la capacidad de realizar cambios en la información de los productos para mantener actualizado el catálogo de la tienda.</t>
-  </si>
-  <si>
-    <t>Implementar una función de actualización de productos permite al administrador modificar detalles como nombre, descripción, precio, disponibilidad, etc.</t>
-  </si>
-  <si>
-    <t>* Diseñar una interfaz de administrador que permita la edición de la información del producto.
-* Proporcionar campos editables para los diferentes atributos del producto, como nombre, descripción, precio, etc.
-* Validar la información actualizada para garantizar su precisión y coherencia.</t>
-  </si>
-  <si>
-    <t>* Iniciar sesión en la aplicación como administrador.
-* Seleccionar el producto que se desea actualizar desde el panel de administración.
-* Modificar uno o más atributos del producto, como el nombre o el precio.
-* Guardar los cambios realizados.
-* Verificar que los cambios se reflejen correctamente en la página de detalles del producto y en el catálogo de la tienda.</t>
-  </si>
-  <si>
     <t>Eliminación de productos</t>
   </si>
   <si>
     <t>El sistema debe permitir al administrador eliminar productos de manera segura y eficiente.</t>
-  </si>
-  <si>
-    <t>El administrador necesita la capacidad de eliminar productos obsoletos, duplicados o incorrectos del catálogo de la tienda para mantener la integridad y relevancia del inventario.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementar una función de eliminación de productos permite al administrador gestionar efectivamente el catálogo de la tienda, eliminando productos innecesarios y manteniendo la calidad del inventario.
-</t>
-  </si>
-  <si>
-    <t>* Diseñar una interfaz de administrador que permita la selección y eliminación de productos.
-* Proporcionar confirmación de eliminación para evitar la eliminación accidental de productos.
-* Implementar controles de seguridad para garantizar que solo el administrador pueda eliminar productos.
-* Actualizar la base de datos del sistema eliminando de manera permanente los productos seleccionados.</t>
-  </si>
-  <si>
-    <t>* Iniciar sesión en la aplicación como administrador.
-* Navegar al panel de administración y seleccionar la opción para administrar productos.
-* Seleccionar el producto que se desea eliminar.
-* Confirmar la eliminación del producto.
-* Verificar que el producto eliminado ya no esté disponible en el catálogo de la tienda.</t>
   </si>
   <si>
     <t xml:space="preserve">El sistema debe permitir la visualización  intuitiva y personalizable del perfil de usuario
@@ -468,15 +317,125 @@
     <t>Visualización del listado de materiales.</t>
   </si>
   <si>
-    <t>*Pruebas de usabilidad para evaluar la facilidad de navegación y comprensión de la interfaz de actualización de datos.
-*Pruebas de funcionamiento para confirmar que los cambios realizados se reflejen correctamente en el perfil del usuario.
-* Evaluación de la seguridad del proceso de actualización para garantizar la protección de los datos del usuario.</t>
+    <t>* Diseñar una interfaz de usuario intuitiva que permita la edición de la información del material.
+* Proporcionar opciones para modificar campos específicos del material.
+* Validar los cambios realizados para garantizar la coherencia y precisión de la información.
+* Guardar los cambios de manera segura y actualizar la base de datos del sistema con la información actualizada del material.</t>
+  </si>
+  <si>
+    <t>* Diseñar una interfaz de usuario que muestre de manera clara y organizada la lista de productos.
+* Incluir información relevante de los productos.
+* Implementar funciones de búsqueda y filtrado para ayudar al administrador a encontrar productos específicos.</t>
+  </si>
+  <si>
+    <t>* Diseñar una interfaz de administrador que permita la edición de la información del producto.
+* Proporcionar campos editables para los diferentes atributos del producto.
+* Validar la información actualizada para garantizar su precisión y coherencia.</t>
+  </si>
+  <si>
+    <t>Ingresa al apartado de perfil, corrobora la información de perfil con la ingresada para verificar que los datos sean correctos.</t>
+  </si>
+  <si>
+    <t>* Diseñar una interfaz que permita al administrador ingresar y confirmar sus credenciales* Desarrollar un proceso de validación que verifique la autenticidad de la actualización de credenciales.</t>
+  </si>
+  <si>
+    <t>Ingresa al formulario los nuevos datos a actualizar, ingresando datos inválidos se puede verificar las validaciones para un llenado correcto de la información.</t>
+  </si>
+  <si>
+    <t>* Diseñar una interfaz de usuario clara y organizada para mostrar el listado de materiales.
+* Organizar los materiales de manera jerárquica o categorizada para una mejor comprensión.</t>
+  </si>
+  <si>
+    <t>Permitirá al administrador encontrar rápidamente los materiales deseados.</t>
+  </si>
+  <si>
+    <t>Implementar una interfaz intuitiva de visualización de listado de productos permite al administrador acceder fácilmente a la información relevante de los productos.</t>
+  </si>
+  <si>
+    <t>Permite al administrador ingresar la información relevante de los nuevos productos de manera eficiente, garantizando así la disponibilidad y precisión del inventario.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar una función de eliminación de productos permitiendo al administrador gestionar efectivamente los productos, eliminando productos innecesarios y manteniendo la calidad del inventario.
+</t>
+  </si>
+  <si>
+    <t>Implementar una funcionalidad de actualización de usuario que permita al usuario modificar tanto su nombre de usuario y su contraseña, garantizando la seguridad y autenticidad del proceso.</t>
+  </si>
+  <si>
+    <t>El administrador necesita la capacidad de agregar nuevos productos al inventario de manera rápida y precisa para mantener actualizado el catálogo de productos disponibles.</t>
+  </si>
+  <si>
+    <t>El administrador necesita la capacidad de encontrar rápidamente productos específicos  para facilitar cualquier proceso.</t>
+  </si>
+  <si>
+    <t>El administrador necesita la capacidad de realizar cambios en la información de los productos para mantener actualizado el inventario.</t>
+  </si>
+  <si>
+    <t>El administrador necesita la capacidad de eliminar productos obsoletos, duplicados o incorrectos  mantener la integridad y relevancia del inventario.</t>
+  </si>
+  <si>
+    <t>En el aplicativo el administrador podrán verificar su información de manera intuitiva y adaptada a sus preferencias.</t>
+  </si>
+  <si>
+    <t>La implementación de una interfaz intuitiva y estructurada permite al administrador acceder al listado de materiales de manera eficaz, facilitando la gestión y el acceso a los recursos necesarios.</t>
+  </si>
+  <si>
+    <t>La implementación de  añadir materiales permiteal administrador contribuir con nuevos recursos al sistema de manera eficiente, asegurando que la base de datos esté actualizada y completa.</t>
+  </si>
+  <si>
+    <t>Implementar una función de actualización de productos permite al administrador modificar nuevos detalles del producto.</t>
+  </si>
+  <si>
+    <t>* Diseñar un formulario claro y fácil de entender para la entrada de información del material.
+* Validar la información ingresada para garantizar su precisión y coherencia.
+* Permitir a los usuarios revisar y confirmar la información antes de añadir el material al sistema.</t>
+  </si>
+  <si>
+    <t>* Diseñar un formulario de entrada de productos.
+* Validar la información ingresada para asegurar su precisión y coherencia.</t>
+  </si>
+  <si>
+    <t>* Diseñar una barra de búsqueda prominente en la interfaz del administrador.
+* Implementar algoritmos de búsqueda eficientes que permitan la búsqueda.
+* Mostrar resultados de búsqueda relevantes de manera clara y ordenada.</t>
+  </si>
+  <si>
+    <t>* Diseñar una interfaz de administrador que permita la eliminación de productos.
+* Proporcionar confirmación de eliminación para evitar la eliminación accidental de productos.
+* Actualizar la base de datos del sistema eliminando de manera permanente los productos seleccionados.</t>
+  </si>
+  <si>
+    <t>Verificar la eficacia de la visualización del listado de materiales corroborando los materiales en el listado.</t>
+  </si>
+  <si>
+    <t>Se ingresa el nombre del material a buscar, ingresando datos inválidos y correctos se puede verificar la busqueda del material deseado,</t>
+  </si>
+  <si>
+    <t>Se modifica el campo de información del material, guarda los cambios realizados y se verificar que los cambios se reflejen correctamente en la interfaz del usuario y en la base de datos del sistema.</t>
+  </si>
+  <si>
+    <t>Se ingresa el material para eliminar, confirma la eliminación del material, se verificar que el material eliminado ya no esté disponible en la base de datos y  comprobamos que las referencias del material eliminado se actualicen correctamente en el sistema.</t>
+  </si>
+  <si>
+    <t>Accede a la página de visualización del listado de productos, se verificar que todos los productos estén listados y sean visibles, realizamos una búsqueda de un producto específico utilizando la función de búsqueda, confirmar visualmente que la información de cada producto sea precisa y esté completa.</t>
+  </si>
+  <si>
+    <t>Ingresar al formulario de añadir productos, ingresar los detalles del nuevo producto, se puede guardar la información del producto y por ultimo se verifica que el nuevo producto aparezca correctamente en la sección de productos de la tienda.</t>
+  </si>
+  <si>
+    <t>Ingresar un término de búsqueda en la barra de búsqueda, se verifica que los resultados de búsqueda coincidan con el término ingresado, probar diferentes términos de búsqueda para asegurar la precisión y la amplitud de los resultados.</t>
+  </si>
+  <si>
+    <t>Ingresa el producto que se desea actualizar desde el panel, modificar el producto, guardar los cambios realizados,  verificar que los cambios se reflejen correctamente en la página de detalles del producto en el inventario.</t>
+  </si>
+  <si>
+    <t>Acceder al panel  y seleccionar la opción para administrar productos,  ingresar el producto que se desea elimina, confirmar la eliminación del producto. Se verifica que el producto eliminado ya no se vea reflejado en le inventario.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -1023,6 +982,17 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1050,6 +1020,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1058,34 +1041,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1415,17 +1374,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="31.69921875" customWidth="1"/>
+    <col min="2" max="2" width="31.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:1">
@@ -1440,39 +1399,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:S1004"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="65" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="65" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.59765625" customWidth="1"/>
-    <col min="4" max="5" width="20.59765625" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.625" customWidth="1"/>
+    <col min="4" max="5" width="20.625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="22.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.8984375" customWidth="1"/>
-    <col min="9" max="9" width="10.59765625" customWidth="1"/>
-    <col min="10" max="10" width="13.69921875" customWidth="1"/>
-    <col min="11" max="12" width="10.59765625" customWidth="1"/>
-    <col min="13" max="15" width="20.59765625" customWidth="1"/>
-    <col min="16" max="26" width="9.3984375" customWidth="1"/>
+    <col min="7" max="7" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
+    <col min="9" max="9" width="10.625" customWidth="1"/>
+    <col min="10" max="10" width="13.75" customWidth="1"/>
+    <col min="11" max="12" width="10.625" customWidth="1"/>
+    <col min="13" max="15" width="20.625" customWidth="1"/>
+    <col min="16" max="26" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="14.4">
+    <row r="1" spans="2:19">
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="2"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="2:19" ht="14.4">
+    <row r="2" spans="2:19">
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="2"/>
@@ -1496,7 +1455,7 @@
       <c r="N3" s="38"/>
       <c r="O3" s="38"/>
     </row>
-    <row r="4" spans="2:19" ht="14.4">
+    <row r="4" spans="2:19">
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1567,7 +1526,7 @@
         <v>24</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I6" s="30">
         <v>4</v>
@@ -1594,22 +1553,22 @@
         <v>19</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I7" s="30">
         <v>1</v>
@@ -1624,34 +1583,34 @@
         <v>25</v>
       </c>
       <c r="M7" s="30" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="N7" s="30"/>
       <c r="O7" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="228" customHeight="1">
       <c r="B8" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="F8" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I8" s="30">
         <v>5</v>
@@ -1666,34 +1625,34 @@
         <v>25</v>
       </c>
       <c r="M8" s="30" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="N8" s="30"/>
       <c r="O8" s="30" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" ht="216">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="135">
       <c r="B9" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I9" s="30">
         <v>1</v>
@@ -1708,34 +1667,34 @@
         <v>25</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="N9" s="30"/>
       <c r="O9" s="30" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" ht="172.8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" ht="180">
       <c r="B10" s="29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="F10" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I10" s="30">
         <v>2</v>
@@ -1750,34 +1709,34 @@
         <v>25</v>
       </c>
       <c r="M10" s="30" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="N10" s="30"/>
       <c r="O10" s="30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" ht="244.8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="165">
       <c r="B11" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I11" s="30">
         <v>2</v>
@@ -1792,34 +1751,34 @@
         <v>25</v>
       </c>
       <c r="M11" s="30" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="N11" s="30"/>
       <c r="O11" s="30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" ht="259.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" ht="240">
       <c r="B12" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="F12" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I12" s="30">
         <v>2</v>
@@ -1834,34 +1793,34 @@
         <v>25</v>
       </c>
       <c r="M12" s="30" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="N12" s="30"/>
       <c r="O12" s="30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" ht="259.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" ht="300">
       <c r="B13" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I13" s="30">
         <v>2</v>
@@ -1876,34 +1835,34 @@
         <v>25</v>
       </c>
       <c r="M13" s="30" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="N13" s="30"/>
       <c r="O13" s="30" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:19" ht="185.25" customHeight="1">
       <c r="B14" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D14" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="30" t="s">
         <v>100</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>106</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I14" s="30">
         <v>1</v>
@@ -1918,34 +1877,34 @@
         <v>25</v>
       </c>
       <c r="M14" s="30" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="N14" s="30"/>
       <c r="O14" s="30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="2:19" ht="187.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" ht="180">
       <c r="B15" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="F15" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="30" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I15" s="30">
         <v>2</v>
@@ -1960,34 +1919,34 @@
         <v>25</v>
       </c>
       <c r="M15" s="30" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="N15" s="30"/>
       <c r="O15" s="30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="2:19" ht="273.60000000000002">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" ht="165">
       <c r="B16" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="30" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I16" s="30">
         <v>2</v>
@@ -2002,40 +1961,40 @@
         <v>25</v>
       </c>
       <c r="M16" s="30" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="N16" s="30"/>
       <c r="O16" s="30" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:19" ht="273.60000000000002">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" ht="165">
       <c r="B17" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="D17" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="30" t="s">
         <v>111</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>112</v>
       </c>
       <c r="F17" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I17" s="30">
         <v>2</v>
@@ -2050,11 +2009,11 @@
         <v>25</v>
       </c>
       <c r="M17" s="30" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="N17" s="30"/>
       <c r="O17" s="30" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="R17" s="2" t="s">
         <v>20</v>
@@ -2063,27 +2022,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="230.4">
+    <row r="18" spans="2:19" ht="210">
       <c r="B18" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="F18" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I18" s="30">
         <v>2</v>
@@ -2098,20 +2057,20 @@
         <v>25</v>
       </c>
       <c r="M18" s="30" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="N18" s="30"/>
       <c r="O18" s="30" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:19" ht="14.4">
+    <row r="19" spans="2:19">
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
@@ -2128,10 +2087,10 @@
       <c r="O19" s="33"/>
       <c r="R19" s="2"/>
       <c r="S19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" ht="13.8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" ht="14.25">
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
@@ -2147,7 +2106,7 @@
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
     </row>
-    <row r="21" spans="2:19" ht="13.8">
+    <row r="21" spans="2:19" ht="14.25">
       <c r="B21" s="33"/>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
@@ -2163,7 +2122,7 @@
       <c r="N21" s="33"/>
       <c r="O21" s="33"/>
     </row>
-    <row r="22" spans="2:19" ht="13.8">
+    <row r="22" spans="2:19" ht="14.25">
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
@@ -2179,7 +2138,7 @@
       <c r="N22" s="33"/>
       <c r="O22" s="33"/>
     </row>
-    <row r="23" spans="2:19" ht="13.8">
+    <row r="23" spans="2:19" ht="14.25">
       <c r="B23" s="33"/>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
@@ -2195,7 +2154,7 @@
       <c r="N23" s="33"/>
       <c r="O23" s="33"/>
     </row>
-    <row r="24" spans="2:19" ht="13.8">
+    <row r="24" spans="2:19" ht="14.25">
       <c r="B24" s="33"/>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
@@ -2211,7 +2170,7 @@
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
     </row>
-    <row r="25" spans="2:19" ht="13.8">
+    <row r="25" spans="2:19" ht="14.25">
       <c r="B25" s="33"/>
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
@@ -2227,7 +2186,7 @@
       <c r="N25" s="33"/>
       <c r="O25" s="33"/>
     </row>
-    <row r="26" spans="2:19" ht="13.8">
+    <row r="26" spans="2:19" ht="14.25">
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
@@ -8062,13 +8021,13 @@
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K19:K23" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K19:K23">
       <formula1>$K$32:$K$34</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L24:L26 L6:L18" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L24:L26 L6:L18">
       <formula1>$S$16:$S$19</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K24:K26 K6:K18" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K24:K26 K6:K18">
       <formula1>$R$16:$R$18</formula1>
     </dataValidation>
   </dataValidations>
@@ -8079,7 +8038,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -8089,47 +8048,47 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" customWidth="1"/>
-    <col min="2" max="2" width="2.59765625" customWidth="1"/>
-    <col min="3" max="15" width="10.59765625" customWidth="1"/>
-    <col min="16" max="16" width="2.59765625" customWidth="1"/>
-    <col min="17" max="26" width="9.3984375" customWidth="1"/>
+    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="2" max="2" width="2.625" customWidth="1"/>
+    <col min="3" max="15" width="10.625" customWidth="1"/>
+    <col min="16" max="16" width="2.625" customWidth="1"/>
+    <col min="17" max="26" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="15" hidden="1" customHeight="1"/>
     <row r="3" spans="2:16" ht="15" hidden="1" customHeight="1"/>
-    <row r="4" spans="2:16" ht="14.4" hidden="1">
+    <row r="4" spans="2:16" hidden="1">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:16" ht="14.4" hidden="1">
+    <row r="5" spans="2:16" hidden="1">
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="2:16" ht="39.75" customHeight="1">
-      <c r="B6" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="58"/>
+      <c r="B6" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="60"/>
     </row>
     <row r="7" spans="2:16" ht="9.75" customHeight="1">
       <c r="C7" s="7"/>
@@ -8169,15 +8128,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="60"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="58"/>
+      <c r="I9" s="60"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -8189,20 +8148,20 @@
     <row r="10" spans="2:16" ht="30" customHeight="1">
       <c r="B10" s="24"/>
       <c r="C10" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="12"/>
-      <c r="E10" s="59" t="str">
+      <c r="E10" s="62" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,5,0)</f>
         <v>Jeanneth Gissela Vela Galeas</v>
       </c>
-      <c r="F10" s="58"/>
+      <c r="F10" s="60"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="59" t="str">
+      <c r="H10" s="62" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,11,0)</f>
         <v>Terminado</v>
       </c>
-      <c r="I10" s="58"/>
+      <c r="I10" s="60"/>
       <c r="J10" s="13"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -8231,18 +8190,18 @@
     <row r="12" spans="2:16" ht="30" customHeight="1">
       <c r="B12" s="24"/>
       <c r="C12" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12" s="12"/>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="58"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="58"/>
+      <c r="H12" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="60"/>
       <c r="J12" s="13"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
@@ -8258,17 +8217,17 @@
         <v>2</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="E13" s="59" t="str">
+      <c r="E13" s="62" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,10,0)</f>
         <v>Alta</v>
       </c>
-      <c r="F13" s="58"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="59" t="str">
+      <c r="H13" s="62" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,7,0)</f>
         <v>Cristian Acalo</v>
       </c>
-      <c r="I13" s="58"/>
+      <c r="I13" s="60"/>
       <c r="J13" s="13"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
@@ -8297,70 +8256,69 @@
     <row r="15" spans="2:16" ht="19.5" customHeight="1">
       <c r="B15" s="24"/>
       <c r="C15" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="42" t="str">
+        <v>38</v>
+      </c>
+      <c r="D15" s="49" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,3,0)</f>
         <v>El administrador necesita la capacidad de incorporar nuevos materiales al sistema para mantener actualizada la base de datos y asegurar la disponibilidad de recursos.</v>
       </c>
-      <c r="E15" s="61"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="10"/>
       <c r="G15" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="42" t="str">
+        <v>39</v>
+      </c>
+      <c r="H15" s="49" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,4,0)</f>
-        <v>La implementación de  añadir materiales permite a los usuarios contribuir con nuevos recursos al sistema de manera eficiente, asegurando que la base de datos esté actualizada y completa.</v>
-      </c>
-      <c r="I15" s="69"/>
-      <c r="J15" s="61"/>
+        <v>La implementación de  añadir materiales permiteal administrador contribuir con nuevos recursos al sistema de manera eficiente, asegurando que la base de datos esté actualizada y completa.</v>
+      </c>
+      <c r="I15" s="63"/>
+      <c r="J15" s="43"/>
       <c r="K15" s="10"/>
       <c r="L15" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="M15" s="42" t="str">
+        <v>40</v>
+      </c>
+      <c r="M15" s="49" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,6,0)</f>
-        <v xml:space="preserve">* Diseñar un formulario claro y fácil de entender para la entrada de información del material.
+        <v>* Diseñar un formulario claro y fácil de entender para la entrada de información del material.
 * Validar la información ingresada para garantizar su precisión y coherencia.
-* Permitir a los usuarios revisar y confirmar la información antes de añadir el material al sistema.
-</v>
-      </c>
-      <c r="N15" s="43"/>
-      <c r="O15" s="44"/>
+* Permitir a los usuarios revisar y confirmar la información antes de añadir el material al sistema.</v>
+      </c>
+      <c r="N15" s="50"/>
+      <c r="O15" s="51"/>
       <c r="P15" s="25"/>
     </row>
     <row r="16" spans="2:16" ht="19.5" customHeight="1">
       <c r="B16" s="24"/>
       <c r="C16" s="40"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="66"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="10"/>
       <c r="G16" s="40"/>
-      <c r="H16" s="65"/>
+      <c r="H16" s="47"/>
       <c r="I16" s="38"/>
-      <c r="J16" s="66"/>
+      <c r="J16" s="48"/>
       <c r="K16" s="10"/>
       <c r="L16" s="40"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="47"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="54"/>
       <c r="P16" s="25"/>
     </row>
     <row r="17" spans="2:16" ht="19.5" customHeight="1">
       <c r="B17" s="24"/>
       <c r="C17" s="41"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="63"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="45"/>
       <c r="F17" s="10"/>
       <c r="G17" s="41"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="63"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="45"/>
       <c r="K17" s="10"/>
       <c r="L17" s="41"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="50"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="57"/>
       <c r="P17" s="25"/>
     </row>
     <row r="18" spans="2:16" ht="9.75" customHeight="1">
@@ -8382,40 +8340,40 @@
     </row>
     <row r="19" spans="2:16" ht="19.5" customHeight="1">
       <c r="B19" s="24"/>
-      <c r="C19" s="60" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="53"/>
+      <c r="C19" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="43"/>
+      <c r="E19" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="67"/>
       <c r="P19" s="25"/>
     </row>
     <row r="20" spans="2:16" ht="19.5" customHeight="1">
       <c r="B20" s="24"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="56"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="70"/>
       <c r="P20" s="25"/>
     </row>
     <row r="21" spans="2:16" ht="9.75" customHeight="1">
@@ -8437,63 +8395,63 @@
     </row>
     <row r="22" spans="2:16" ht="19.5" customHeight="1">
       <c r="B22" s="24"/>
-      <c r="C22" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="42" t="str">
+      <c r="C22" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="43"/>
+      <c r="E22" s="49" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,12,0)</f>
         <v>Verificar la funcionalidad de añadir materiales mediante pruebas de ingreso de datos y comprobación de que los nuevos materiales se reflejen correctamente en la base de datos del sistema.</v>
       </c>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="44"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="51"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="64" t="s">
+      <c r="J22" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="61"/>
-      <c r="L22" s="42">
+      <c r="K22" s="43"/>
+      <c r="L22" s="49">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,13,0)</f>
         <v>0</v>
       </c>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="44"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="51"/>
       <c r="P22" s="25"/>
     </row>
     <row r="23" spans="2:16" ht="19.5" customHeight="1">
       <c r="B23" s="24"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="54"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="54"/>
       <c r="P23" s="25"/>
     </row>
     <row r="24" spans="2:16" ht="19.5" customHeight="1">
       <c r="B24" s="24"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="50"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="57"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="63"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="50"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="57"/>
       <c r="P24" s="25"/>
     </row>
     <row r="25" spans="2:16" ht="9.75" customHeight="1">
@@ -9510,6 +9468,11 @@
     <row r="1020" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:O17"/>
+    <mergeCell ref="E19:O20"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C19:D20"/>
     <mergeCell ref="C22:D24"/>
@@ -9526,11 +9489,6 @@
     <mergeCell ref="D15:E17"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="H15:J17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:O17"/>
-    <mergeCell ref="E19:O20"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -9553,7 +9511,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Formato descripción HU'!$B$6:$B$10</xm:f>
           </x14:formula1>

</xml_diff>